<commit_message>
the start of applications
</commit_message>
<xml_diff>
--- a/datasets.xlsx
+++ b/datasets.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +526,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>transactions_10302022.xlsx</t>
+          <t>transactions_11122022.xlsx</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -535,6 +535,66 @@
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>d67af7eb-76b5-4943-9d4a-00b152c16171</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11/04/2022</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>calories</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>calories_11042022.xlsx</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>b27aaea9-db0f-4987-9771-700e2a6a43f5</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11/06/2022</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>calendar</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>calendar.xlsx</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated headers df with default view and editable
</commit_message>
<xml_diff>
--- a/datasets.xlsx
+++ b/datasets.xlsx
@@ -6,13 +6,12 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId4"/>
-    <sheet name="headers" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -26,22 +25,37 @@
     <t>name</t>
   </si>
   <si>
-    <t>model</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
     <t>status</t>
   </si>
   <si>
-    <t>default_table</t>
-  </si>
-  <si>
-    <t>07cab2e2-624b-402c-bcc6-4a4319a91fd7</t>
-  </si>
-  <si>
-    <t>10/24/2022</t>
+    <t>5c2956e4-5226-11ed-bdc3-0242ac120002</t>
+  </si>
+  <si>
+    <t>calories</t>
+  </si>
+  <si>
+    <t>calories_11042022.xlsx</t>
+  </si>
+  <si>
+    <t>archive</t>
+  </si>
+  <si>
+    <t>66f1301a-5226-11ed-bdc3-0242ac120002</t>
+  </si>
+  <si>
+    <t>contacts</t>
+  </si>
+  <si>
+    <t>contacts_11272022.xlsx</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>7347d8c8-5226-11ed-bdc3-0242ac120002</t>
   </si>
   <si>
     <t>donations</t>
@@ -50,106 +64,25 @@
     <t>donations.xlsx</t>
   </si>
   <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>['date','name']</t>
-  </si>
-  <si>
-    <t>da09485c-9737-43e3-8a36-9d0ccd4712b8</t>
-  </si>
-  <si>
-    <t>10/30/2022</t>
+    <t>7dae0814-5226-11ed-bdc3-0242ac120002</t>
+  </si>
+  <si>
+    <t>stocks</t>
+  </si>
+  <si>
+    <t>stocks.xlsx</t>
+  </si>
+  <si>
+    <t>eb79c6aa-7fb0-4112-b1b3-86b0d506e5ec</t>
+  </si>
+  <si>
+    <t>10/23/2022</t>
   </si>
   <si>
     <t>transactions</t>
   </si>
   <si>
     <t>transactions_11242022.xlsx</t>
-  </si>
-  <si>
-    <t>[ 'Amount', 'Description', 'Expense', 'Transaction Date', 'Reviewed', 'Account' ]</t>
-  </si>
-  <si>
-    <t>d67af7eb-76b5-4943-9d4a-00b152c16171</t>
-  </si>
-  <si>
-    <t>11/04/2022</t>
-  </si>
-  <si>
-    <t>calories</t>
-  </si>
-  <si>
-    <t>calories_11042022.xlsx</t>
-  </si>
-  <si>
-    <t>[ 'date', 'excercise', 'consumption', 'fat' ]</t>
-  </si>
-  <si>
-    <t>8e5a1dc4-796c-440a-a9b2-d41a7acae24b</t>
-  </si>
-  <si>
-    <t>11/15/2022</t>
-  </si>
-  <si>
-    <t>stocks</t>
-  </si>
-  <si>
-    <t>stocks.xlsx</t>
-  </si>
-  <si>
-    <t>['symbol','qty']</t>
-  </si>
-  <si>
-    <t>dtype</t>
-  </si>
-  <si>
-    <t>alias</t>
-  </si>
-  <si>
-    <t>editable</t>
-  </si>
-  <si>
-    <t>picklist</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>Created</t>
-  </si>
-  <si>
-    <t>Modified</t>
-  </si>
-  <si>
-    <t>str</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>object</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>['archive','active']</t>
-  </si>
-  <si>
-    <t>table</t>
-  </si>
-  <si>
-    <t>Table</t>
   </si>
 </sst>
 </file>
@@ -196,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -279,13 +212,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -295,7 +315,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -304,22 +324,43 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1432,15 +1473,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="8.85156" style="1" customWidth="1"/>
-    <col min="8" max="8" width="58.8516" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.8516" style="1" customWidth="1"/>
+    <col min="2" max="3" width="8.85156" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1462,317 +1506,120 @@
       <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s" s="2">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s" s="5">
+        <v>8</v>
+      </c>
       <c r="F2" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s" s="5">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s" s="6">
-        <v>15</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" t="s" s="8">
-        <v>16</v>
-      </c>
-      <c r="E3" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="E3" t="s" s="8">
+        <v>12</v>
+      </c>
       <c r="F3" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s" s="8">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s" s="8">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s" s="6">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="E4" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="E4" t="s" s="8">
+        <v>16</v>
+      </c>
       <c r="F4" t="s" s="8">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s" s="8">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s" s="8">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s" s="6">
-        <v>25</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" t="s" s="8">
-        <v>26</v>
-      </c>
-      <c r="E5" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="E5" t="s" s="8">
+        <v>19</v>
+      </c>
       <c r="F5" t="s" s="8">
-        <v>27</v>
-      </c>
-      <c r="G5" t="s" s="8">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s" s="8">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="5" width="8.85156" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" t="b" s="10">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s" s="6">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="D3" t="b" s="11">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s" s="6">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s" s="8">
-        <v>36</v>
-      </c>
-      <c r="D4" t="b" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s" s="6">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s" s="8">
-        <v>38</v>
-      </c>
-      <c r="D5" t="b" s="11">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s" s="6">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s" s="8">
-        <v>39</v>
-      </c>
-      <c r="D6" t="b" s="11">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="B6" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s" s="8">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s" s="6">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="D7" t="b" s="11">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s" s="6">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s" s="8">
-        <v>42</v>
-      </c>
-      <c r="D8" t="b" s="11">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s" s="8">
-        <v>43</v>
-      </c>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s" s="6">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s" s="8">
-        <v>45</v>
-      </c>
-      <c r="D9" t="b" s="11">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed datasets date format curruptions
</commit_message>
<xml_diff>
--- a/datasets.xlsx
+++ b/datasets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -569,7 +569,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10/23/2022</t>
+          <t>2022-10-23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -597,7 +597,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>11/28/2022</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -625,7 +625,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>11/28/2022</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -653,7 +653,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>12/10/2022</t>
+          <t>2022-12-10</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -681,7 +681,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>12/10/2022</t>
+          <t>2022-12-10</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -709,7 +709,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>12/10/2022</t>
+          <t>2022-12-10</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -724,6 +724,34 @@
         </is>
       </c>
       <c r="F11" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>0f6bad26-cd71-4c67-ae5e-66bd7c37fc02</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2022-12-10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>methods</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>methods.xlsx</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>active</t>
         </is>

</xml_diff>

<commit_message>
Metrics support, taxes app update, and taxes2022 sheet created, addrecord updated
</commit_message>
<xml_diff>
--- a/datasets.xlsx
+++ b/datasets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -757,6 +757,34 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>bccf28a2-848e-4783-ad20-4da0c98f73cd</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2023-01-30</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>taxes2022</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>taxes2022.xlsx</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>